<commit_message>
added awesome environments and templates for future labs
</commit_message>
<xml_diff>
--- a/Geometrical Optics/data.xlsx
+++ b/Geometrical Optics/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cmailcarletonca-my.sharepoint.com/personal/camilarestrepo_cmail_carleton_ca/Documents/23-24/W24/phys2202/Geometrical Optics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1656" documentId="11_F25DC773A252ABDACC10487E79187C425BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{511A2F71-E6CC-4F5C-9223-28DAFAC0FA7E}"/>
+  <xr:revisionPtr revIDLastSave="1663" documentId="11_F25DC773A252ABDACC10487E79187C425BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FFA5B4B-4876-4A1D-9F36-F71E0A65F8F8}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="827" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="827" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apparatus (Measurement)" sheetId="4" r:id="rId1"/>
@@ -228,9 +228,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="166" formatCode="0.0000000000"/>
-    <numFmt numFmtId="167" formatCode="0.000000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,13 +321,25 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -336,26 +348,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1244,8 +1242,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Magnification!$L$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.0029632264</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1267,6 +1276,42 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
+            <c:numRef>
+              <c:f>Magnification!$L$13:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000000000</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.8779462975220878E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7818733134893033E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6387312979919255E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5512156542592543E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6492171563303043E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2884866237956837E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.092181517668473E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5711659622605935E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9632263608617062E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Magnification!$K$13:$K$21</c:f>
               <c:numCache>
@@ -1301,47 +1346,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Magnification!$L$13:$L$21</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000000000</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2.8779462975220878E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.7818733134893033E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6387312979919255E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5512156542592543E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.6492171563303043E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2884866237956837E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.092181517668473E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.5711659622605935E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.9632263608617062E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C574-482E-917B-FC25B0844A50}"/>
+              <c16:uniqueId val="{00000015-D445-4DF2-B325-343A33F09B10}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3774,38 +3783,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="11"/>
+      <c r="A1" s="18"/>
       <c r="B1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5">
         <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="11"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
@@ -3818,7 +3827,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
@@ -3934,16 +3943,16 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="12"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="12"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="6" t="s">
         <v>33</v>
       </c>
@@ -3955,7 +3964,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="12"/>
+      <c r="A16" s="19"/>
       <c r="B16">
         <f>'Apparatus (Measurement)'!B4</f>
         <v>0.5</v>
@@ -3997,24 +4006,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
@@ -4023,7 +4032,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
@@ -4113,16 +4122,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="12"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="12"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
@@ -4134,7 +4143,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="12"/>
+      <c r="A12" s="19"/>
       <c r="C12">
         <f>STDEV(D4:D8)</f>
         <v>1.1401754250991381</v>
@@ -4174,45 +4183,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="10" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="11"/>
+      <c r="K2" s="18"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="6" t="s">
         <v>39</v>
       </c>
@@ -4273,11 +4282,11 @@
         <f t="shared" ref="H4:H13" si="1">1/F4</f>
         <v>2.5641025641025641E-3</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="10">
         <f>E4*F4/(E4+F4)</f>
         <v>197.46835443037975</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="10">
         <f>(SQRT(1/2) / (E4+F4)) * SQRT(E4^2 + F4^2)</f>
         <v>0.50004005607857416</v>
       </c>
@@ -4311,11 +4320,11 @@
         <f t="shared" si="1"/>
         <v>2.2123893805309734E-3</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="10">
         <f t="shared" ref="I5:I13" si="4">E5*F5/(E5+F5)</f>
         <v>197.2568578553616</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="10">
         <f t="shared" ref="J5:J13" si="5">(SQRT(1/2) / (E5+F5)) * SQRT(E5^2 + F5^2)</f>
         <v>0.50402759660107832</v>
       </c>
@@ -4349,11 +4358,11 @@
         <f t="shared" si="1"/>
         <v>2.7972027972027972E-3</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="10">
         <f t="shared" si="4"/>
         <v>199.22600619195046</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="10">
         <f t="shared" si="5"/>
         <v>0.50326979612131206</v>
       </c>
@@ -4387,11 +4396,11 @@
         <f t="shared" si="1"/>
         <v>3.003003003003003E-3</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="10">
         <f t="shared" si="4"/>
         <v>199.87995198079233</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="10">
         <f t="shared" si="5"/>
         <v>0.50994909241392983</v>
       </c>
@@ -4425,11 +4434,11 @@
         <f t="shared" si="1"/>
         <v>2.3584905660377358E-3</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="10">
         <f t="shared" si="4"/>
         <v>197.58186397984886</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="10">
         <f t="shared" si="5"/>
         <v>0.50115500854989847</v>
       </c>
@@ -4463,11 +4472,11 @@
         <f t="shared" si="1"/>
         <v>2.4875621890547263E-3</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="10">
         <f t="shared" si="4"/>
         <v>197.95454545454547</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="10">
         <f t="shared" si="5"/>
         <v>0.50005738880937123</v>
       </c>
@@ -4501,11 +4510,11 @@
         <f t="shared" si="1"/>
         <v>2.5773195876288659E-3</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="10">
         <f t="shared" si="4"/>
         <v>199.34837092731829</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="10">
         <f t="shared" si="5"/>
         <v>0.50018997527866882</v>
       </c>
@@ -4539,11 +4548,11 @@
         <f t="shared" si="1"/>
         <v>2.7027027027027029E-3</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="10">
         <f t="shared" si="4"/>
         <v>198.875</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="10">
         <f t="shared" si="5"/>
         <v>0.50140427800328946</v>
       </c>
@@ -4577,11 +4586,11 @@
         <f t="shared" si="1"/>
         <v>2.0554984583761563E-3</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="10">
         <f t="shared" si="4"/>
         <v>196.62584200857319</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="10">
         <f t="shared" si="5"/>
         <v>0.50910167631787617</v>
       </c>
@@ -4615,17 +4624,17 @@
         <f t="shared" si="1"/>
         <v>1.8587360594795538E-3</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="10">
         <f t="shared" si="4"/>
         <v>196.6745283018868</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="10">
         <f t="shared" si="5"/>
         <v>0.51775717301650126</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="L14" s="15">
+      <c r="L14" s="10">
         <f>AVERAGE(I4:I13)</f>
         <v>198.08913211306566</v>
       </c>
@@ -4639,35 +4648,35 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" s="12"/>
-      <c r="B31" s="10" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A32" s="12"/>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11" t="s">
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="12"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="6" t="s">
         <v>11</v>
       </c>
@@ -4691,7 +4700,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="12"/>
+      <c r="A34" s="19"/>
       <c r="B34">
         <f>10*(SUM(C37:C46)) - SUM(A37:A46)^2</f>
         <v>1.089549575920975E-5</v>
@@ -4905,16 +4914,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="B1:D1"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4926,8 +4935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AE9DB3-2B61-4BF2-A04B-ABAB2D8D8BA5}">
   <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" zoomScale="61" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4937,27 +4946,27 @@
     <col min="4" max="4" width="20.1328125" customWidth="1"/>
     <col min="5" max="5" width="15.1328125" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="8" max="9" width="14.265625" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.86328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.19921875" style="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.86328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.86328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.265625" style="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.19921875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.19921875" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="11.19921875" style="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="11.19921875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A1" s="11"/>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="5" t="s">
         <v>52</v>
       </c>
@@ -4966,7 +4975,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5">
         <v>152.47</v>
       </c>
@@ -4975,26 +4984,26 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A5" s="11"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A6" s="11"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
@@ -5003,7 +5012,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="6" t="s">
         <v>54</v>
       </c>
@@ -5021,7 +5030,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A8" s="11"/>
+      <c r="A8" s="18"/>
       <c r="B8">
         <v>19.5</v>
       </c>
@@ -5044,51 +5053,51 @@
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="18" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="4"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="19" t="s">
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="P11" s="19"/>
+      <c r="P11" s="23"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="4"/>
@@ -5110,46 +5119,46 @@
       <c r="G12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="21" t="s">
+      <c r="L12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="22" t="s">
+      <c r="O12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="P12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="17" t="s">
+      <c r="Q12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="S12" s="25" t="s">
+      <c r="S12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="T12" s="25" t="s">
+      <c r="T12" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="U12" s="25" t="s">
+      <c r="U12" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="V12" s="25" t="s">
+      <c r="V12" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5175,56 +5184,56 @@
       <c r="G13">
         <v>-15</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="11">
         <f>(D13-C13) +$B$3 +Magnification!$E$8/2</f>
         <v>450.47</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="11">
         <f>(F13-E13) +$B$3 +Magnification!$E$8/2</f>
         <v>347.47</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="11">
         <f>$B$8/G13</f>
         <v>-1.3</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="11">
         <f t="shared" ref="K13:K21" si="0">1 / H13</f>
         <v>2.2199036561813216E-3</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="11">
         <f t="shared" ref="L13:L21" si="1">1/I13</f>
         <v>2.8779462975220878E-3</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="11">
         <f>H13*I13/(H13+I13)</f>
         <v>196.16112853096723</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="11">
         <f>(SQRT(1/2)/G13) * SQRT(1 + (J13)^2)</f>
         <v>-7.7316090031621362E-2</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="11">
         <f>SQRT(5/4 + 1/2500)</f>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P13" s="17">
+      <c r="P13" s="11">
         <f>O13/H13^2</f>
         <v>5.5105219349470169E-6</v>
       </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="11">
         <f>O13/I13^2</f>
         <v>9.2616817565025278E-6</v>
       </c>
-      <c r="S13" s="25">
+      <c r="S13" s="16">
         <v>2.8779462999999998E-3</v>
       </c>
-      <c r="T13" s="25">
+      <c r="T13" s="16">
         <v>2.2199036999999999E-3</v>
       </c>
-      <c r="U13" s="25">
+      <c r="U13" s="16">
         <v>1.1714499999999999E-5</v>
       </c>
-      <c r="V13" s="25">
+      <c r="V13" s="16">
         <v>6.9699E-6</v>
       </c>
     </row>
@@ -5250,56 +5259,56 @@
       <c r="G14">
         <v>-16</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="11">
         <f>(D14-C14) +$B$3 +Magnification!$E$8/2</f>
         <v>430.97</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="11">
         <f>(F14-E14) +$B$3 +Magnification!$E$8/2</f>
         <v>359.47</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="11">
         <f t="shared" ref="J14:J21" si="2">$B$8/G14</f>
         <v>-1.21875</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="11">
         <f t="shared" si="0"/>
         <v>2.3203471239297397E-3</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="11">
         <f t="shared" si="1"/>
         <v>2.7818733134893033E-3</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="11">
         <f t="shared" ref="M14:M21" si="3">H14*I14/(H14+I14)</f>
         <v>195.99309991903246</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="11">
         <f t="shared" ref="N14:N21" si="4">(SQRT(1/2)/G14) * SQRT(1 + (J14)^2)</f>
         <v>-6.9672105397410047E-2</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="11">
         <f t="shared" ref="O14:O21" si="5">SQRT(5/4 + 1/2500)</f>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P14" s="17">
+      <c r="P14" s="11">
         <f t="shared" ref="P14:P21" si="6">O14/H14^2</f>
         <v>6.0204700869266086E-6</v>
       </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="11">
         <f t="shared" ref="Q14:Q21" si="7">O14/I14^2</f>
         <v>8.6536470740241776E-6</v>
       </c>
-      <c r="S14" s="25">
+      <c r="S14" s="16">
         <v>2.7818732999999999E-3</v>
       </c>
-      <c r="T14" s="25">
+      <c r="T14" s="16">
         <v>2.3203471E-3</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14" s="16">
         <v>1.09454E-5</v>
       </c>
-      <c r="V14" s="25">
+      <c r="V14" s="16">
         <v>7.6148999999999997E-6</v>
       </c>
     </row>
@@ -5325,56 +5334,56 @@
       <c r="G15">
         <v>-17.5</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="11">
         <f>(D15-C15) +$B$3 +Magnification!$E$8/2</f>
         <v>411.47</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="11">
         <f>(F15-E15) +$B$3 +Magnification!$E$8/2</f>
         <v>378.97</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="11">
         <f t="shared" si="2"/>
         <v>-1.1142857142857143</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="11">
         <f t="shared" si="0"/>
         <v>2.430310836756021E-3</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="11">
         <f t="shared" si="1"/>
         <v>2.6387312979919255E-3</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="11">
         <f t="shared" si="3"/>
         <v>197.27592973533729</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="11">
         <f t="shared" si="4"/>
         <v>-6.0496350411914805E-2</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P15" s="17">
+      <c r="P15" s="11">
         <f t="shared" si="6"/>
         <v>6.6046244712013276E-6</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="11">
         <f t="shared" si="7"/>
         <v>7.786007523501136E-6</v>
       </c>
-      <c r="S15" s="25">
+      <c r="S15" s="16">
         <v>2.6387313000000002E-3</v>
       </c>
-      <c r="T15" s="25">
+      <c r="T15" s="16">
         <v>2.4303108E-3</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15" s="16">
         <v>9.8479999999999996E-6</v>
       </c>
-      <c r="V15" s="25">
+      <c r="V15" s="16">
         <v>8.3537999999999995E-6</v>
       </c>
     </row>
@@ -5400,56 +5409,56 @@
       <c r="G16">
         <v>-19</v>
       </c>
-      <c r="H16" s="17">
+      <c r="H16" s="11">
         <f>(D16-C16) +$B$3 +Magnification!$E$8/2</f>
         <v>390.97</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="11">
         <f>(F16-E16) +$B$3 +Magnification!$E$8/2</f>
         <v>391.97</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="11">
         <f t="shared" si="2"/>
         <v>-1.0263157894736843</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="11">
         <f t="shared" si="0"/>
         <v>2.5577410031460213E-3</v>
       </c>
-      <c r="L16" s="17">
+      <c r="L16" s="11">
         <f t="shared" si="1"/>
         <v>2.5512156542592543E-3</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="11">
         <f t="shared" si="3"/>
         <v>195.73468069072982</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="11">
         <f t="shared" si="4"/>
         <v>-5.332859642154697E-2</v>
       </c>
-      <c r="O16" s="17">
+      <c r="O16" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P16" s="17">
+      <c r="P16" s="11">
         <f t="shared" si="6"/>
         <v>7.3153921834388804E-6</v>
       </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="11">
         <f t="shared" si="7"/>
         <v>7.2781135110307306E-6</v>
       </c>
-      <c r="S16" s="25">
+      <c r="S16" s="16">
         <v>2.5512157000000001E-3</v>
       </c>
-      <c r="T16" s="25">
+      <c r="T16" s="16">
         <v>2.5577410000000001E-3</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16" s="16">
         <v>9.2056000000000004E-6</v>
       </c>
-      <c r="V16" s="25">
+      <c r="V16" s="16">
         <v>9.2528000000000006E-6</v>
       </c>
     </row>
@@ -5475,56 +5484,56 @@
       <c r="G17">
         <v>-21</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="11">
         <f>(D17-C17) +$B$3 +Magnification!$E$8/2</f>
         <v>371.47</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="11">
         <f>(F17-E17) +$B$3 +Magnification!$E$8/2</f>
         <v>377.47</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="11">
         <f t="shared" si="2"/>
         <v>-0.9285714285714286</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="11">
         <f t="shared" si="0"/>
         <v>2.6920074299405065E-3</v>
       </c>
-      <c r="L17" s="17">
+      <c r="L17" s="11">
         <f t="shared" si="1"/>
         <v>2.6492171563303043E-3</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="11">
         <f t="shared" si="3"/>
         <v>187.22298301599594</v>
       </c>
-      <c r="N17" s="17">
+      <c r="N17" s="11">
         <f t="shared" si="4"/>
         <v>-4.594985063301462E-2</v>
       </c>
-      <c r="O17" s="17">
+      <c r="O17" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P17" s="17">
+      <c r="P17" s="11">
         <f t="shared" si="6"/>
         <v>8.1035812503049185E-6</v>
       </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="11">
         <f t="shared" si="7"/>
         <v>7.8480109487431465E-6</v>
       </c>
-      <c r="S17" s="25">
+      <c r="S17" s="16">
         <v>2.6492171999999998E-3</v>
       </c>
-      <c r="T17" s="25">
+      <c r="T17" s="16">
         <v>2.6920073999999999E-3</v>
       </c>
-      <c r="U17" s="25">
+      <c r="U17" s="16">
         <v>9.9264000000000004E-6</v>
       </c>
-      <c r="V17" s="25">
+      <c r="V17" s="16">
         <v>1.0249699999999999E-5</v>
       </c>
     </row>
@@ -5550,56 +5559,56 @@
       <c r="G18">
         <v>-25</v>
       </c>
-      <c r="H18" s="17">
+      <c r="H18" s="11">
         <f>(D18-C18) +$B$3 +Magnification!$E$8/2</f>
         <v>351.47</v>
       </c>
-      <c r="I18" s="17">
+      <c r="I18" s="11">
         <f>(F18-E18) +$B$3 +Magnification!$E$8/2</f>
         <v>436.97</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="11">
         <f t="shared" si="2"/>
         <v>-0.78</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K18" s="11">
         <f t="shared" si="0"/>
         <v>2.8451930463481946E-3</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18" s="11">
         <f t="shared" si="1"/>
         <v>2.2884866237956837E-3</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="11">
         <f t="shared" si="3"/>
         <v>194.792052534118</v>
       </c>
-      <c r="N18" s="17">
+      <c r="N18" s="11">
         <f t="shared" si="4"/>
         <v>-3.5870879554312576E-2</v>
       </c>
-      <c r="O18" s="17">
+      <c r="O18" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P18" s="17">
+      <c r="P18" s="11">
         <f t="shared" si="6"/>
         <v>9.0520711675716873E-6</v>
       </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="11">
         <f t="shared" si="7"/>
         <v>5.8562719921062435E-6</v>
       </c>
-      <c r="S18" s="25">
+      <c r="S18" s="16">
         <v>2.2884865999999999E-3</v>
       </c>
-      <c r="T18" s="25">
+      <c r="T18" s="16">
         <v>2.8451930000000002E-3</v>
       </c>
-      <c r="U18" s="25">
+      <c r="U18" s="16">
         <v>7.4072E-6</v>
       </c>
-      <c r="V18" s="25">
+      <c r="V18" s="16">
         <v>1.1449399999999999E-5</v>
       </c>
     </row>
@@ -5625,56 +5634,56 @@
       <c r="G19">
         <v>-27.5</v>
       </c>
-      <c r="H19" s="17">
+      <c r="H19" s="11">
         <f>(D19-C19) +$B$3 +Magnification!$E$8/2</f>
         <v>330.97</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="11">
         <f>(F19-E19) +$B$3 +Magnification!$E$8/2</f>
         <v>477.97</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="11">
         <f t="shared" si="2"/>
         <v>-0.70909090909090911</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K19" s="11">
         <f t="shared" si="0"/>
         <v>3.0214218811372628E-3</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19" s="11">
         <f t="shared" si="1"/>
         <v>2.092181517668473E-3</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19" s="11">
         <f t="shared" si="3"/>
         <v>195.55681620392119</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19" s="11">
         <f t="shared" si="4"/>
         <v>-3.1521315546605533E-2</v>
       </c>
-      <c r="O19" s="17">
+      <c r="O19" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P19" s="17">
+      <c r="P19" s="11">
         <f t="shared" si="6"/>
         <v>1.0208154221256143E-5</v>
       </c>
-      <c r="Q19" s="17">
+      <c r="Q19" s="11">
         <f t="shared" si="7"/>
         <v>4.8946676114802146E-6</v>
       </c>
-      <c r="S19" s="25">
+      <c r="S19" s="16">
         <v>2.0921815E-3</v>
       </c>
-      <c r="T19" s="25">
+      <c r="T19" s="16">
         <v>3.0214219000000001E-3</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19" s="16">
         <v>6.1909000000000003E-6</v>
       </c>
-      <c r="V19" s="25">
+      <c r="V19" s="16">
         <v>1.29116E-5</v>
       </c>
     </row>
@@ -5700,56 +5709,56 @@
       <c r="G20">
         <v>-33</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="11">
         <f>(D20-C20) +$B$3 +Magnification!$E$8/2</f>
         <v>309.97000000000003</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="11">
         <f>(F20-E20) +$B$3 +Magnification!$E$8/2</f>
         <v>636.47</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="11">
         <f t="shared" si="2"/>
         <v>-0.59090909090909094</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="11">
         <f t="shared" si="0"/>
         <v>3.2261186566441909E-3</v>
       </c>
-      <c r="L20" s="17">
+      <c r="L20" s="11">
         <f t="shared" si="1"/>
         <v>1.5711659622605935E-3</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="11">
         <f t="shared" si="3"/>
         <v>208.45125512446643</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="11">
         <f t="shared" si="4"/>
         <v>-2.4888858126160682E-2</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O20" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P20" s="17">
+      <c r="P20" s="11">
         <f t="shared" si="6"/>
         <v>1.1638182305890472E-5</v>
       </c>
-      <c r="Q20" s="17">
+      <c r="Q20" s="11">
         <f t="shared" si="7"/>
         <v>2.7603783116326329E-6</v>
       </c>
-      <c r="S20" s="25">
+      <c r="S20" s="16">
         <v>1.5711659999999999E-3</v>
       </c>
-      <c r="T20" s="25">
+      <c r="T20" s="16">
         <v>3.2261186999999998E-3</v>
       </c>
-      <c r="U20" s="25">
+      <c r="U20" s="16">
         <v>3.4914000000000001E-6</v>
       </c>
-      <c r="V20" s="25">
+      <c r="V20" s="16">
         <v>1.4720400000000001E-5</v>
       </c>
     </row>
@@ -5775,56 +5784,56 @@
       <c r="G21">
         <v>-14</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="11">
         <f>(D21-C21) +$B$3 +Magnification!$E$8/2</f>
         <v>479.47</v>
       </c>
-      <c r="I21" s="17">
+      <c r="I21" s="11">
         <f>(F21-E21) +$B$3 +Magnification!$E$8/2</f>
         <v>337.47</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="11">
         <f t="shared" si="2"/>
         <v>-1.3928571428571428</v>
       </c>
-      <c r="K21" s="17">
+      <c r="K21" s="11">
         <f t="shared" si="0"/>
         <v>2.0856362233299267E-3</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="11">
         <f t="shared" si="1"/>
         <v>2.9632263608617062E-3</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="11">
         <f t="shared" si="3"/>
         <v>198.0644121967342</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="11">
         <f t="shared" si="4"/>
         <v>-8.6603291820244677E-2</v>
       </c>
-      <c r="O21" s="17">
+      <c r="O21" s="11">
         <f t="shared" si="5"/>
         <v>1.1182128598795491</v>
       </c>
-      <c r="P21" s="17">
+      <c r="P21" s="11">
         <f t="shared" si="6"/>
         <v>4.8640900284859102E-6</v>
       </c>
-      <c r="Q21" s="17">
+      <c r="Q21" s="11">
         <f t="shared" si="7"/>
         <v>9.8187033616310687E-6</v>
       </c>
-      <c r="S21" s="25">
+      <c r="S21" s="16">
         <v>2.9632263999999999E-3</v>
       </c>
-      <c r="T21" s="25">
+      <c r="T21" s="16">
         <v>2.0856362000000002E-3</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21" s="16">
         <v>1.2418999999999999E-5</v>
       </c>
-      <c r="V21" s="25">
+      <c r="V21" s="16">
         <v>6.1523000000000004E-6</v>
       </c>
     </row>
@@ -5838,40 +5847,40 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="23"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="23" t="s">
+      <c r="H39" s="12"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="23"/>
-      <c r="P39" s="23"/>
-      <c r="Q39" s="23"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+      <c r="Q39" s="12"/>
       <c r="R39" s="2"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A40" s="3"/>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
-      <c r="H40" s="20"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="19" t="s">
+      <c r="H40" s="13"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
       <c r="R40" s="4"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.45">
@@ -5888,36 +5897,36 @@
       <c r="E41" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" t="s">
         <v>57</v>
       </c>
-      <c r="G41" s="16" t="s">
+      <c r="G41" t="s">
         <v>12</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H41" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="J41" s="24"/>
-      <c r="K41" s="21" t="s">
+      <c r="J41" s="15"/>
+      <c r="K41" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L41" s="21" t="s">
+      <c r="L41" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M41" s="21"/>
-      <c r="N41" s="21" t="s">
+      <c r="M41" s="14"/>
+      <c r="N41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O41" s="21" t="s">
+      <c r="O41" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="P41" s="16" t="s">
+      <c r="P41" t="s">
         <v>57</v>
       </c>
-      <c r="Q41" s="16" t="s">
+      <c r="Q41" t="s">
         <v>12</v>
       </c>
-      <c r="R41" s="17" t="s">
+      <c r="R41" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5947,24 +5956,24 @@
         <f>F42*SQRT(9/B42)</f>
         <v>1.5923956625995745E-4</v>
       </c>
-      <c r="H42" s="17">
+      <c r="H42" s="11">
         <f>F42*SQRT(SUM(D45:D53)/B42)</f>
         <v>6.2980956429664808E-2</v>
       </c>
-      <c r="J42" s="24"/>
-      <c r="K42" s="17">
+      <c r="J42" s="15"/>
+      <c r="K42" s="11">
         <f>8*(SUM(N45:N52)) - SUM(K45:K52)^2</f>
         <v>1.2204937984024253E-5</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L42" s="11">
         <f>(1/K42)*(8 * SUM(O45:O52) - SUM(K45:K52)*SUM(L45:L52))</f>
         <v>-0.84849863040062989</v>
       </c>
-      <c r="N42" s="17">
+      <c r="N42" s="11">
         <f>(1/K42)*(SUM(N45:N52)*SUM(L45:L52)-SUM(K45:K52)*SUM(O45:O52))</f>
         <v>4.6846376363384864E-3</v>
       </c>
-      <c r="O42" s="17">
+      <c r="O42" s="11">
         <f>1/N42</f>
         <v>213.46368227993835</v>
       </c>
@@ -5976,7 +5985,7 @@
         <f>P42*SQRT(8/K42)</f>
         <v>1.5500764794193944</v>
       </c>
-      <c r="R42" s="17">
+      <c r="R42" s="11">
         <f>P42*SQRT(SUM(N45:N53)/K42)</f>
         <v>3.8889881148040568E-3</v>
       </c>
@@ -5994,16 +6003,16 @@
       <c r="E44" t="s">
         <v>47</v>
       </c>
-      <c r="K44" s="17" t="s">
+      <c r="K44" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="L44" s="17" t="s">
+      <c r="L44" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="N44" s="17" t="s">
+      <c r="N44" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="O44" s="17" t="s">
+      <c r="O44" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6024,19 +6033,19 @@
         <f>B45*C45</f>
         <v>-585.6110000000001</v>
       </c>
-      <c r="K45" s="17">
-        <f t="shared" ref="K45:K49" si="10">L13</f>
+      <c r="K45" s="11">
+        <f t="shared" ref="K45:K48" si="10">L13</f>
         <v>2.8779462975220878E-3</v>
       </c>
-      <c r="L45" s="17">
-        <f t="shared" ref="L45:L49" si="11">K13</f>
+      <c r="L45" s="11">
+        <f t="shared" ref="L45:L48" si="11">K13</f>
         <v>2.2199036561813216E-3</v>
       </c>
-      <c r="N45" s="17">
+      <c r="N45" s="11">
         <f>K45^2</f>
         <v>8.2825748914210937E-6</v>
       </c>
-      <c r="O45" s="17">
+      <c r="O45" s="11">
         <f>K45*L45</f>
         <v>6.3887635081627802E-6</v>
       </c>
@@ -6058,27 +6067,27 @@
         <f>B46*C46</f>
         <v>-525.24468750000005</v>
       </c>
-      <c r="H46" s="17">
+      <c r="H46" s="11">
         <f>G42/C42^2</f>
         <v>6.6916076612874553</v>
       </c>
-      <c r="K46" s="17">
+      <c r="K46" s="11">
         <f t="shared" si="10"/>
         <v>2.7818733134893033E-3</v>
       </c>
-      <c r="L46" s="17">
+      <c r="L46" s="11">
         <f t="shared" si="11"/>
         <v>2.3203471239297397E-3</v>
       </c>
-      <c r="N46" s="17">
-        <f t="shared" ref="N46:N49" si="13">K46^2</f>
+      <c r="N46" s="11">
+        <f t="shared" ref="N46:N48" si="13">K46^2</f>
         <v>7.7388191323039559E-6</v>
       </c>
-      <c r="O46" s="17">
+      <c r="O46" s="11">
         <f>K46*L46</f>
         <v>6.4549117420918E-6</v>
       </c>
-      <c r="R46" s="17">
+      <c r="R46" s="11">
         <f>R42/N42^2</f>
         <v>177.2085244949364</v>
       </c>
@@ -6100,20 +6109,20 @@
         <f t="shared" ref="E47:E53" si="14">B47*C47</f>
         <v>-458.49514285714292</v>
       </c>
-      <c r="K47" s="17">
+      <c r="K47" s="11">
         <f t="shared" si="10"/>
         <v>2.6387312979919255E-3</v>
       </c>
-      <c r="L47" s="17">
+      <c r="L47" s="11">
         <f t="shared" si="11"/>
         <v>2.430310836756021E-3</v>
       </c>
-      <c r="N47" s="17">
+      <c r="N47" s="11">
         <f t="shared" si="13"/>
         <v>6.9629028630021521E-6</v>
       </c>
-      <c r="O47" s="17">
-        <f t="shared" ref="O47:O49" si="15">K47*L47</f>
+      <c r="O47" s="11">
+        <f t="shared" ref="O47:O48" si="15">K47*L47</f>
         <v>6.4129372687970581E-6</v>
       </c>
     </row>
@@ -6134,19 +6143,19 @@
         <f t="shared" si="14"/>
         <v>-401.25868421052638</v>
       </c>
-      <c r="K48" s="17">
+      <c r="K48" s="11">
         <f t="shared" si="10"/>
         <v>2.5512156542592543E-3</v>
       </c>
-      <c r="L48" s="17">
+      <c r="L48" s="11">
         <f t="shared" si="11"/>
         <v>2.5577410031460213E-3</v>
       </c>
-      <c r="N48" s="17">
+      <c r="N48" s="11">
         <f t="shared" si="13"/>
         <v>6.508701314537475E-6</v>
       </c>
-      <c r="O48" s="17">
+      <c r="O48" s="11">
         <f t="shared" si="15"/>
         <v>6.5253488867668982E-6</v>
       </c>
@@ -6168,19 +6177,19 @@
         <f t="shared" si="14"/>
         <v>-344.93642857142862</v>
       </c>
-      <c r="K49" s="17">
+      <c r="K49" s="11">
         <f>L18</f>
         <v>2.2884866237956837E-3</v>
       </c>
-      <c r="L49" s="17">
+      <c r="L49" s="11">
         <f>K18</f>
         <v>2.8451930463481946E-3</v>
       </c>
-      <c r="N49" s="17">
+      <c r="N49" s="11">
         <f>K49^2</f>
         <v>5.2371710272917669E-6</v>
       </c>
-      <c r="O49" s="17">
+      <c r="O49" s="11">
         <f>K49*L49</f>
         <v>6.5111862286843357E-6</v>
       </c>
@@ -6202,19 +6211,19 @@
         <f t="shared" si="14"/>
         <v>-274.14660000000003</v>
       </c>
-      <c r="K50" s="17">
+      <c r="K50" s="11">
         <f>L19</f>
         <v>2.092181517668473E-3</v>
       </c>
-      <c r="L50" s="17">
+      <c r="L50" s="11">
         <f>K19</f>
         <v>3.0214218811372628E-3</v>
       </c>
-      <c r="N50" s="17">
+      <c r="N50" s="11">
         <f>K50^2</f>
         <v>4.3772235028735554E-6</v>
       </c>
-      <c r="O50" s="17">
+      <c r="O50" s="11">
         <f>K50*L50</f>
         <v>6.3213630167944913E-6</v>
       </c>
@@ -6236,19 +6245,19 @@
         <f t="shared" si="14"/>
         <v>-234.68781818181822</v>
       </c>
-      <c r="K51" s="17">
+      <c r="K51" s="11">
         <f>L20</f>
         <v>1.5711659622605935E-3</v>
       </c>
-      <c r="L51" s="17">
+      <c r="L51" s="11">
         <f>K20</f>
         <v>3.2261186566441909E-3</v>
       </c>
-      <c r="N51" s="17">
+      <c r="N51" s="11">
         <f>K51^2</f>
         <v>2.4685624809662569E-6</v>
       </c>
-      <c r="O51" s="17">
+      <c r="O51" s="11">
         <f>K51*L51</f>
         <v>5.0687678235332237E-6</v>
       </c>
@@ -6270,19 +6279,19 @@
         <f t="shared" si="14"/>
         <v>-183.16409090909093</v>
       </c>
-      <c r="K52" s="17">
+      <c r="K52" s="11">
         <f>L21</f>
         <v>2.9632263608617062E-3</v>
       </c>
-      <c r="L52" s="17">
+      <c r="L52" s="11">
         <f>K21</f>
         <v>2.0856362233299267E-3</v>
       </c>
-      <c r="N52" s="17">
+      <c r="N52" s="11">
         <f>K52^2</f>
         <v>8.7807104657057104E-6</v>
       </c>
-      <c r="O52" s="17">
+      <c r="O52" s="11">
         <f>K52*L52</f>
         <v>6.1802122361392917E-6</v>
       </c>
@@ -6324,7 +6333,7 @@
         <f>$L$42*K45+$N$42</f>
         <v>2.2427041445244314E-3</v>
       </c>
-      <c r="M55" s="26">
+      <c r="M55" s="17">
         <f>(L45-L55)^2</f>
         <v>5.1986226868428484E-10</v>
       </c>
@@ -6342,7 +6351,7 @@
         <f t="shared" ref="L56:L63" si="16">$L$42*K46+$N$42</f>
         <v>2.3242219398947506E-3</v>
       </c>
-      <c r="M56" s="26">
+      <c r="M56" s="17">
         <f t="shared" ref="M56:M63" si="17">(L46-L56)^2</f>
         <v>1.5014198762703362E-11</v>
       </c>
@@ -6360,7 +6369,7 @@
         <f t="shared" si="16"/>
         <v>2.4456777439970613E-3</v>
       </c>
-      <c r="M57" s="26">
+      <c r="M57" s="17">
         <f t="shared" si="17"/>
         <v>2.3614183815473588E-10</v>
       </c>
@@ -6378,7 +6387,7 @@
         <f t="shared" si="16"/>
         <v>2.5199346478428624E-3</v>
       </c>
-      <c r="M58" s="26">
+      <c r="M58" s="17">
         <f t="shared" si="17"/>
         <v>1.4293205013086907E-9</v>
       </c>
@@ -6396,7 +6405,7 @@
         <f t="shared" si="16"/>
         <v>2.7428598703576872E-3</v>
       </c>
-      <c r="M59" s="26">
+      <c r="M59" s="17">
         <f t="shared" si="17"/>
         <v>1.047207890830415E-8</v>
       </c>
@@ -6414,7 +6423,7 @@
         <f t="shared" si="16"/>
         <v>2.9094244840472761E-3</v>
       </c>
-      <c r="M60" s="26">
+      <c r="M60" s="17">
         <f t="shared" si="17"/>
         <v>1.2543416954932167E-8</v>
       </c>
@@ -6432,7 +6441,7 @@
         <f t="shared" si="16"/>
         <v>3.351505469228285E-3</v>
       </c>
-      <c r="M61" s="26">
+      <c r="M61" s="17">
         <f t="shared" si="17"/>
         <v>1.5721852769998738E-8</v>
       </c>
@@ -6450,7 +6459,7 @@
         <f t="shared" si="16"/>
         <v>2.170344127580286E-3</v>
       </c>
-      <c r="M62" s="26">
+      <c r="M62" s="17">
         <f t="shared" si="17"/>
         <v>7.1754290424880437E-9</v>
       </c>
@@ -6468,7 +6477,7 @@
         <f t="shared" si="16"/>
         <v>4.6846376363384864E-3</v>
       </c>
-      <c r="M63" s="26">
+      <c r="M63" s="17">
         <f t="shared" si="17"/>
         <v>2.1945829783799039E-5</v>
       </c>
@@ -6485,6 +6494,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H10:P10"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="K40:O40"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A5:A8"/>
@@ -6493,11 +6507,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H10:P10"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="K40:O40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6509,7 +6518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0461AD-CCF8-490F-BEA4-C59996F02263}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="118" workbookViewId="0">
+    <sheetView zoomScale="118" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -6521,25 +6530,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="11"/>
+      <c r="A1" s="18"/>
       <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="11"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="11"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="5">
         <v>1.51502</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -6547,13 +6556,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="11"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="11"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
@@ -6567,41 +6576,41 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="21"/>
+      <c r="D10" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11" t="s">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11" t="s">
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>

</xml_diff>